<commit_message>
rectifying local uncommitted stage changes
</commit_message>
<xml_diff>
--- a/bicc_template.xlsx
+++ b/bicc_template.xlsx
@@ -6144,8 +6144,8 @@
   </sheetPr>
   <dimension ref="A1:L259"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
-      <selection activeCell="I194" sqref="I194"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A188" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
+      <selection activeCell="G195" sqref="G195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9501,7 +9501,7 @@
       </c>
       <c r="I194" s="232"/>
     </row>
-    <row r="195" spans="1:9" s="24" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:9" s="24" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="303"/>
       <c r="B195" s="304" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
further change on way to fixing validation
</commit_message>
<xml_diff>
--- a/bicc_template.xlsx
+++ b/bicc_template.xlsx
@@ -90,14 +90,18 @@
     <definedName function="false" hidden="false" name="YN_2" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Summary!$A$1:$L$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Concept" vbProcedure="false">Dropdown!$AD$2:$AD$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Other" vbProcedure="false">Dropdown!$AD$2:$AD$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -4923,9 +4927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1882800</xdr:colOff>
+      <xdr:colOff>1882440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1034640</xdr:rowOff>
+      <xdr:rowOff>1034280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4939,7 +4943,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="322200" y="83880"/>
-          <a:ext cx="1560600" cy="950760"/>
+          <a:ext cx="1560240" cy="950400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4965,9 +4969,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1560600</xdr:colOff>
+      <xdr:colOff>1560240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>997920</xdr:rowOff>
+      <xdr:rowOff>997560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4981,7 +4985,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1560600" cy="997920"/>
+          <a:ext cx="1560240" cy="997560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5007,9 +5011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1550160</xdr:colOff>
+      <xdr:colOff>1549800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>960480</xdr:rowOff>
+      <xdr:rowOff>960120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5023,7 +5027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1550160" cy="960480"/>
+          <a:ext cx="1549800" cy="960120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5049,9 +5053,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1560600</xdr:colOff>
+      <xdr:colOff>1560240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>960480</xdr:rowOff>
+      <xdr:rowOff>960120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5065,7 +5069,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1560600" cy="960480"/>
+          <a:ext cx="1560240" cy="960120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5091,9 +5095,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1560600</xdr:colOff>
+      <xdr:colOff>1560240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>960480</xdr:rowOff>
+      <xdr:rowOff>960120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5107,7 +5111,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1560600" cy="960480"/>
+          <a:ext cx="1560240" cy="960120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6085,7 +6089,7 @@
   <dataValidations count="22">
     <dataValidation allowBlank="true" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H35:K35 I36:K38 C47:K47" type="textLength">
       <formula1>7001</formula1>
-      <formula2> </formula2>
+      <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B26:C26 G26:G27 K27" type="textLength">
       <formula1>5001</formula1>
@@ -9766,10 +9770,6 @@
       <formula1>Dropdown!$X$2:$X$90</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B192" type="list">
-      <formula1>Dropdown!$AG$2:$AG$11</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D15" type="list">
       <formula1>Dropdown!$V$2:$V$3</formula1>
       <formula2>0</formula2>
@@ -9784,6 +9784,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B193" type="none">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B192" type="list">
+      <formula1>Dropdown!$AG$2:$AG$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -12026,7 +12030,7 @@
   </sheetPr>
   <dimension ref="A1:AR90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="87" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="AE10" colorId="64" zoomScale="100" zoomScaleNormal="87" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AF2" activeCellId="0" sqref="AF2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
hiding rows in template
</commit_message>
<xml_diff>
--- a/bicc_template.xlsx
+++ b/bicc_template.xlsx
@@ -94,18 +94,24 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Concept" vbProcedure="false">Dropdown!$AD$2:$AD$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Other" vbProcedure="false">Dropdown!$AD$2:$AD$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
@@ -114,6 +120,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -4940,9 +4948,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1881360</xdr:colOff>
+      <xdr:colOff>1880640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1033200</xdr:rowOff>
+      <xdr:rowOff>1032480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4956,7 +4964,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="322200" y="83880"/>
-          <a:ext cx="1559160" cy="949320"/>
+          <a:ext cx="1558440" cy="948600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4982,9 +4990,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1559160</xdr:colOff>
+      <xdr:colOff>1558440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>996480</xdr:rowOff>
+      <xdr:rowOff>995760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4998,7 +5006,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1559160" cy="996480"/>
+          <a:ext cx="1558440" cy="995760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5024,9 +5032,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1548720</xdr:colOff>
+      <xdr:colOff>1548000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>959040</xdr:rowOff>
+      <xdr:rowOff>958320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5040,7 +5048,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1548720" cy="959040"/>
+          <a:ext cx="1548000" cy="958320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5066,9 +5074,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1559160</xdr:colOff>
+      <xdr:colOff>1558440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>959040</xdr:rowOff>
+      <xdr:rowOff>958320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5082,7 +5090,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1559160" cy="959040"/>
+          <a:ext cx="1558440" cy="958320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5108,9 +5116,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1559160</xdr:colOff>
+      <xdr:colOff>1558440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>959040</xdr:rowOff>
+      <xdr:rowOff>958320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5124,7 +5132,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1559160" cy="959040"/>
+          <a:ext cx="1558440" cy="958320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6207,8 +6215,8 @@
   </sheetPr>
   <dimension ref="A1:L198"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A172" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B197" activeCellId="0" sqref="B197"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6596,7 +6604,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" s="19" customFormat="true" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="78" t="s">
         <v>100</v>
       </c>
@@ -6614,7 +6622,7 @@
       <c r="H27" s="82"/>
       <c r="I27" s="82"/>
     </row>
-    <row r="28" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" s="19" customFormat="true" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="78"/>
       <c r="B28" s="79" t="s">
         <v>102</v>
@@ -6630,7 +6638,7 @@
       <c r="H28" s="83"/>
       <c r="I28" s="83"/>
     </row>
-    <row r="29" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" s="19" customFormat="true" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="78" t="s">
         <v>103</v>
       </c>
@@ -6648,7 +6656,7 @@
       <c r="H29" s="84"/>
       <c r="I29" s="84"/>
     </row>
-    <row r="30" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" s="19" customFormat="true" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="78"/>
       <c r="B30" s="79" t="s">
         <v>102</v>
@@ -6664,7 +6672,7 @@
       <c r="H30" s="83"/>
       <c r="I30" s="83"/>
     </row>
-    <row r="31" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" s="19" customFormat="true" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="78" t="s">
         <v>104</v>
       </c>
@@ -6682,7 +6690,7 @@
       <c r="H31" s="83"/>
       <c r="I31" s="83"/>
     </row>
-    <row r="32" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" s="19" customFormat="true" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="78"/>
       <c r="B32" s="79" t="s">
         <v>102</v>
@@ -6698,7 +6706,7 @@
       <c r="H32" s="83"/>
       <c r="I32" s="83"/>
     </row>
-    <row r="33" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" s="19" customFormat="true" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="78" t="s">
         <v>105</v>
       </c>
@@ -6716,7 +6724,7 @@
       <c r="H33" s="83"/>
       <c r="I33" s="83"/>
     </row>
-    <row r="34" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" s="19" customFormat="true" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="78"/>
       <c r="B34" s="79" t="s">
         <v>102</v>
@@ -7515,7 +7523,7 @@
       <c r="H79" s="10"/>
       <c r="I79" s="10"/>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="78" t="s">
         <v>100</v>
       </c>
@@ -7533,7 +7541,7 @@
       <c r="H80" s="10"/>
       <c r="I80" s="10"/>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="78"/>
       <c r="B81" s="79" t="s">
         <v>102</v>
@@ -7549,7 +7557,7 @@
       <c r="H81" s="10"/>
       <c r="I81" s="10"/>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="78" t="s">
         <v>103</v>
       </c>
@@ -7567,7 +7575,7 @@
       <c r="H82" s="10"/>
       <c r="I82" s="10"/>
     </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="78"/>
       <c r="B83" s="79" t="s">
         <v>102</v>
@@ -7583,7 +7591,7 @@
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="78" t="s">
         <v>104</v>
       </c>
@@ -7601,7 +7609,7 @@
       <c r="H84" s="10"/>
       <c r="I84" s="10"/>
     </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="78"/>
       <c r="B85" s="79" t="s">
         <v>102</v>
@@ -7617,7 +7625,7 @@
       <c r="H85" s="10"/>
       <c r="I85" s="10"/>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="78" t="s">
         <v>105</v>
       </c>
@@ -7635,7 +7643,7 @@
       <c r="H86" s="10"/>
       <c r="I86" s="10"/>
     </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="78"/>
       <c r="B87" s="79" t="s">
         <v>102</v>
@@ -8676,7 +8684,7 @@
       <c r="H143" s="10"/>
       <c r="I143" s="10"/>
     </row>
-    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="78" t="s">
         <v>100</v>
       </c>
@@ -8694,7 +8702,7 @@
       <c r="H144" s="10"/>
       <c r="I144" s="10"/>
     </row>
-    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="78"/>
       <c r="B145" s="144" t="s">
         <v>102</v>
@@ -8710,7 +8718,7 @@
       <c r="H145" s="10"/>
       <c r="I145" s="10"/>
     </row>
-    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="78" t="s">
         <v>103</v>
       </c>
@@ -8728,7 +8736,7 @@
       <c r="H146" s="10"/>
       <c r="I146" s="10"/>
     </row>
-    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="78"/>
       <c r="B147" s="144" t="s">
         <v>102</v>
@@ -8744,7 +8752,7 @@
       <c r="H147" s="10"/>
       <c r="I147" s="10"/>
     </row>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="78" t="s">
         <v>104</v>
       </c>
@@ -8762,7 +8770,7 @@
       <c r="H148" s="10"/>
       <c r="I148" s="10"/>
     </row>
-    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="78"/>
       <c r="B149" s="144" t="s">
         <v>102</v>
@@ -8778,7 +8786,7 @@
       <c r="H149" s="10"/>
       <c r="I149" s="10"/>
     </row>
-    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="78" t="s">
         <v>105</v>
       </c>
@@ -8796,7 +8804,7 @@
       <c r="H150" s="10"/>
       <c r="I150" s="10"/>
     </row>
-    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="78"/>
       <c r="B151" s="144" t="s">
         <v>102</v>
@@ -9730,7 +9738,7 @@
     <cfRule type="beginsWith" priority="3" operator="beginsWith" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Amber" dxfId="0"/>
     <cfRule type="beginsWith" priority="4" operator="beginsWith" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Red" dxfId="0"/>
   </conditionalFormatting>
-  <dataValidations count="17">
+  <dataValidations count="18">
     <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C27:E36 H27:I28 H30:I31 H33:I34 H36:I36 C38:E71 H38:I71 C80:E89 C91:E124 C144:E187" type="decimal">
       <formula1>-1</formula1>
       <formula2>0</formula2>
@@ -9755,7 +9763,7 @@
       <formula1>Dropdown!$R$2:$R$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6 C141" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C141" type="list">
       <formula1>Dropdown!$J$2:$J$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9797,6 +9805,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B192" type="list">
       <formula1>Dropdown!$AG$2:$AG$11</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6" type="none">
+      <formula1>Dropdown!$J$2:$J$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
removed three yes/no and a rag verif in f&b to test errors in excel
</commit_message>
<xml_diff>
--- a/bicc_template.xlsx
+++ b/bicc_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,6 +96,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">Summary!$A$1:$L$49</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
@@ -104,6 +105,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Finance &amp; Benefits'!$A$1:$I$197</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
@@ -112,6 +114,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">Resource!$A$1:$M$39</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Concept" vbProcedure="false">Dropdown!$AD$2:$AD$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Other" vbProcedure="false">Dropdown!$AD$2:$AD$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
@@ -122,6 +125,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Approval &amp; Project milestones'!$A$1:$L$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -4963,9 +4967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1880640</xdr:colOff>
+      <xdr:colOff>1880280</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1032480</xdr:rowOff>
+      <xdr:rowOff>1032120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4979,7 +4983,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="322200" y="83880"/>
-          <a:ext cx="1558440" cy="948600"/>
+          <a:ext cx="1558080" cy="948240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5005,9 +5009,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1558440</xdr:colOff>
+      <xdr:colOff>1558080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>995760</xdr:rowOff>
+      <xdr:rowOff>995400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5021,7 +5025,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1558440" cy="995760"/>
+          <a:ext cx="1558080" cy="995400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5047,9 +5051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1548000</xdr:colOff>
+      <xdr:colOff>1547640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>958320</xdr:rowOff>
+      <xdr:rowOff>957960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5063,7 +5067,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1548000" cy="958320"/>
+          <a:ext cx="1547640" cy="957960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5089,9 +5093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1558440</xdr:colOff>
+      <xdr:colOff>1558080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>958320</xdr:rowOff>
+      <xdr:rowOff>957960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5105,7 +5109,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1558440" cy="958320"/>
+          <a:ext cx="1558080" cy="957960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5131,9 +5135,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1558440</xdr:colOff>
+      <xdr:colOff>1558080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>958320</xdr:rowOff>
+      <xdr:rowOff>957960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5147,7 +5151,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1558440" cy="958320"/>
+          <a:ext cx="1558080" cy="957960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6230,8 +6234,8 @@
   </sheetPr>
   <dimension ref="A1:L198"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A133" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="68" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9753,7 +9757,7 @@
     <cfRule type="beginsWith" priority="3" operator="beginsWith" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Amber" dxfId="0"/>
     <cfRule type="beginsWith" priority="4" operator="beginsWith" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Red" dxfId="0"/>
   </conditionalFormatting>
-  <dataValidations count="18">
+  <dataValidations count="19">
     <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C27:E36 H27:I28 H30:I31 H33:I34 H36:I36 C38:E71 H38:I71 C80:E89 C91:E124 C144:E187" type="decimal">
       <formula1>-1</formula1>
       <formula2>0</formula2>
@@ -9776,10 +9780,6 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18 E18" type="list">
       <formula1>Dropdown!$R$2:$R$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C141" type="list">
-      <formula1>Dropdown!$J$2:$J$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C9 E9:E10" type="list">
@@ -9810,7 +9810,7 @@
       <formula1>dropdown!#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H29:I29 C37:F37 H37:I37 C90:F90 F139:F141" type="list">
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H29:I29 C37:F37 H37:I37 C90:F90" type="list">
       <formula1>Dropdown!$V$2:$V$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9823,6 +9823,14 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6" type="none">
+      <formula1>Dropdown!$J$2:$J$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F139:F141" type="none">
+      <formula1>Dropdown!$V$2:$V$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C141" type="none">
       <formula1>Dropdown!$J$2:$J$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10646,7 +10654,7 @@
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="71" zoomScalePageLayoutView="77" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="71" zoomScalePageLayoutView="77" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>